<commit_message>
Added 5V to 3.3V level translator
</commit_message>
<xml_diff>
--- a/Accessories/ExpansionBoard_IO_Converter/REV20201011A/IO_Converter_bom_qty_1.xlsx
+++ b/Accessories/ExpansionBoard_IO_Converter/REV20201011A/IO_Converter_bom_qty_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brandt\Documents\AMDC-Hardware\Accessories\ExpansionBoard_IO_Converter\REV20201011A\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485AF2C9-8F38-4F6C-97B7-03FF1E3A28C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88DCE30-5F87-40A6-81E0-D17507B07C1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EA6FF13C-72BD-4A19-826D-D7080B6F4704}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5C6210A-7EF2-4FE7-9EA1-CB20F92DAE5D}"/>
   </bookViews>
   <sheets>
     <sheet name="IO_Converter_bom_qty_1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Quantity</t>
   </si>
@@ -63,7 +63,7 @@
     <t>311-1341-1-ND</t>
   </si>
   <si>
-    <t>C1, C2</t>
+    <t>C1, C2, C3, C4, C5, C6, C7, C8, C9, C10, C11, C12</t>
   </si>
   <si>
     <t>0.1uF</t>
@@ -96,13 +96,31 @@
     <t>U1</t>
   </si>
   <si>
+    <t>SN74LVC1T45DBVR</t>
+  </si>
+  <si>
+    <t>296-16843-1-ND</t>
+  </si>
+  <si>
+    <t>U2, U3, U5, U6</t>
+  </si>
+  <si>
     <t>AM26C32IPWR</t>
   </si>
   <si>
     <t>296-30088-1-ND</t>
   </si>
   <si>
-    <t>U2</t>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>TLV73333PDBVR</t>
+  </si>
+  <si>
+    <t>296-40673-1-ND</t>
+  </si>
+  <si>
+    <t>U7</t>
   </si>
 </sst>
 </file>
@@ -484,14 +502,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB2B8805-CB65-4B9B-98F3-B88A85BBC9C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{810702A5-A768-4025-8D8B-4C3C6649655A}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,9 +540,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
@@ -539,7 +557,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -598,7 +616,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>19</v>
@@ -611,6 +629,42 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>